<commit_message>
added ch4 to GNFR C
</commit_message>
<xml_diff>
--- a/output/2019/sector_totals_2019.xlsx
+++ b/output/2019/sector_totals_2019.xlsx
@@ -509,7 +509,7 @@
         <v>394.9544215286256</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>79.37230812425607</v>
       </c>
       <c r="G3" t="n">
         <v>4.449361053106772</v>
@@ -834,7 +834,7 @@
         <v>7910.739008973328</v>
       </c>
       <c r="F16" t="n">
-        <v>4414.235496376621</v>
+        <v>4493.607804500877</v>
       </c>
       <c r="G16" t="n">
         <v>49.32103049837363</v>

</xml_diff>